<commit_message>
Adjusting name of method in RoleRepository. Adjusting tests in module daoRepository.
</commit_message>
<xml_diff>
--- a/daoRepository/src/test/resources/documentsList/documentsList.xlsx
+++ b/daoRepository/src/test/resources/documentsList/documentsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\document-archive\daoRepository\src\test\resources\documentsList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D989C54D-22DA-40E2-B03B-0DCD889FEF96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4026BB-3544-43F0-BD96-987C23A32F79}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>USER_NAME</t>
   </si>
@@ -42,13 +42,16 @@
     <t>PATH_TO_DOCUMENT</t>
   </si>
   <si>
-    <t>/documentsList/documents/testDocumentMariusz.docx</t>
-  </si>
-  <si>
     <t>/documentsList/documents/testDocumentUser123.docx</t>
   </si>
   <si>
     <t>/documentsList/documents/testDocumentUser1234.pdf</t>
+  </si>
+  <si>
+    <t>/documentsList/documents/testDocumentMariusz1.docx</t>
+  </si>
+  <si>
+    <t>/documentsList/documents/testDocumentMariusz2.docx</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,23 +394,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>